<commit_message>
added output for the engineer
</commit_message>
<xml_diff>
--- a/1st & last gens.xlsx
+++ b/1st & last gens.xlsx
@@ -380,142 +380,142 @@
         <v>0</v>
       </c>
       <c r="B1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="n">
-        <v>113.3528079545626</v>
+        <v>114.1620489728746</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="n">
-        <v>63.77067407143974</v>
+        <v>67.63156526669685</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D3" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="B4" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="B6" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="B7" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="B8" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="B9" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D9" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
         <v>15</v>
-      </c>
-      <c r="D10" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="B11" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="B12" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D13" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="B14" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D14" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="B15" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="B16" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D16" t="n">
         <v>11</v>
@@ -523,34 +523,34 @@
     </row>
     <row r="17" spans="1:7">
       <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="n">
         <v>10</v>
-      </c>
-      <c r="D17" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="B18" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="B19" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="B20" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D20" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -558,13 +558,13 @@
         <v>4</v>
       </c>
       <c r="B21" t="n">
-        <v>0.7306931568125248</v>
+        <v>0.6956393348003318</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8282612107788319</v>
+        <v>0.7941561180693337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>